<commit_message>
Time measurement and more
- some new .csv/.xlsx with time measurements
- added oPar to MCTSWrapperAgent & MctseWrapperAgent, so that AgentBase.trainAgent works correctly for RubiksCube (epiLength)
- fixed a bug in GameBoardOthelloGui.updateBoard
- larger fonts in Othello's GameStats & Legend
</commit_message>
<xml_diff>
--- a/agents/ConnectFour/csv/mCompeteMCTS-vs-MWrap-25runs-normF.xlsx
+++ b/agents/ConnectFour/csv/mCompeteMCTS-vs-MWrap-25runs-normF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wolfgang\Documents\GitHub\GBG\agents\ConnectFour\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE2E42E-6A44-488E-B550-65B8842C5F4D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2897EC09-75C3-48A6-8122-DC69B9C1A196}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8592" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,9 +21,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="15">
-  <si>
-    <t>TDNTuple3Agt: USESYM:true, P:4, NORMALIZE:false, sigmoid:tanh, lambda:0.0, horizon:1, AFTERSTATE:false, learnFromRM: true</t>
-  </si>
   <si>
     <t>TDNTuple3Agt: alpha_init-&gt;final:3.7-&gt;3.7, epsilon_init-&gt;final:0.1-&gt;0.0, gamma: 1.0, fixed n-tuple, mode=1, evalQ: 0, evalT: -1</t>
   </si>
@@ -65,6 +62,9 @@
   </si>
   <si>
     <t>TCL-base</t>
+  </si>
+  <si>
+    <t>TDNTuple3Agt: USESYM:true, P:4, NORMALIZE:false, sigmoid:tanh, lambda:0.0, horizon:1, AFTERSTATE:false, learnFromRM: true, 250.000 episodes</t>
   </si>
 </sst>
 </file>
@@ -908,52 +908,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>7</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>8</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" t="s">
         <v>9</v>
-      </c>
-      <c r="I3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -982,7 +982,7 @@
         <v>0.92</v>
       </c>
       <c r="I4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -1014,7 +1014,7 @@
         <v>0.88</v>
       </c>
       <c r="I5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -1046,7 +1046,7 @@
         <v>0.84</v>
       </c>
       <c r="I6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -1078,7 +1078,7 @@
         <v>0.96</v>
       </c>
       <c r="I7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -1110,7 +1110,7 @@
         <v>0.98</v>
       </c>
       <c r="I8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -1142,7 +1142,7 @@
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -1174,7 +1174,7 @@
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -1206,7 +1206,7 @@
         <v>0.88</v>
       </c>
       <c r="I11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -1238,7 +1238,7 @@
         <v>0.96</v>
       </c>
       <c r="I12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -1270,7 +1270,7 @@
         <v>0.98</v>
       </c>
       <c r="I13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -1302,7 +1302,7 @@
         <v>0.8</v>
       </c>
       <c r="I14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J14">
         <v>0</v>
@@ -1334,7 +1334,7 @@
         <v>0.98</v>
       </c>
       <c r="I15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -1366,7 +1366,7 @@
         <v>1</v>
       </c>
       <c r="I16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J16">
         <v>0</v>
@@ -1398,7 +1398,7 @@
         <v>0.98</v>
       </c>
       <c r="I17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J17">
         <v>0</v>
@@ -1430,7 +1430,7 @@
         <v>0.8</v>
       </c>
       <c r="I18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J18">
         <v>0</v>
@@ -1462,7 +1462,7 @@
         <v>0.9</v>
       </c>
       <c r="I19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J19">
         <v>0</v>
@@ -1494,7 +1494,7 @@
         <v>0.9</v>
       </c>
       <c r="I20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J20">
         <v>0</v>
@@ -1526,7 +1526,7 @@
         <v>0.92</v>
       </c>
       <c r="I21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J21">
         <v>0</v>
@@ -1558,7 +1558,7 @@
         <v>1</v>
       </c>
       <c r="I22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J22">
         <v>0</v>
@@ -1590,7 +1590,7 @@
         <v>0.98</v>
       </c>
       <c r="I23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J23">
         <v>0</v>
@@ -1622,7 +1622,7 @@
         <v>0.96</v>
       </c>
       <c r="I24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J24">
         <v>0</v>
@@ -1654,7 +1654,7 @@
         <v>0.76</v>
       </c>
       <c r="I25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J25">
         <v>0</v>
@@ -1686,7 +1686,7 @@
         <v>0.9</v>
       </c>
       <c r="I26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J26">
         <v>0</v>
@@ -1718,7 +1718,7 @@
         <v>0.88</v>
       </c>
       <c r="I27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J27">
         <v>0</v>
@@ -1750,7 +1750,7 @@
         <v>0.96</v>
       </c>
       <c r="I28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J28">
         <v>0</v>
@@ -1782,7 +1782,7 @@
         <v>1</v>
       </c>
       <c r="I29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J29">
         <v>0</v>
@@ -1814,7 +1814,7 @@
         <v>1</v>
       </c>
       <c r="I30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J30">
         <v>0</v>
@@ -1846,7 +1846,7 @@
         <v>1</v>
       </c>
       <c r="I31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J31">
         <v>0</v>
@@ -1878,7 +1878,7 @@
         <v>0.84</v>
       </c>
       <c r="I32" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J32">
         <v>0</v>
@@ -1910,7 +1910,7 @@
         <v>0.84</v>
       </c>
       <c r="I33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J33">
         <v>0</v>
@@ -1942,7 +1942,7 @@
         <v>0.9</v>
       </c>
       <c r="I34" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J34">
         <v>0</v>
@@ -1974,7 +1974,7 @@
         <v>0.94</v>
       </c>
       <c r="I35" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J35">
         <v>0</v>
@@ -2006,7 +2006,7 @@
         <v>1</v>
       </c>
       <c r="I36" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J36">
         <v>0</v>
@@ -2038,7 +2038,7 @@
         <v>1</v>
       </c>
       <c r="I37" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J37">
         <v>0</v>
@@ -2070,7 +2070,7 @@
         <v>0.98</v>
       </c>
       <c r="I38" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J38">
         <v>0</v>
@@ -2102,7 +2102,7 @@
         <v>0.77</v>
       </c>
       <c r="I39" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J39">
         <v>0</v>
@@ -2134,7 +2134,7 @@
         <v>0.77</v>
       </c>
       <c r="I40" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J40">
         <v>0</v>
@@ -2166,7 +2166,7 @@
         <v>0.8</v>
       </c>
       <c r="I41" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J41">
         <v>0</v>
@@ -2198,7 +2198,7 @@
         <v>0.8</v>
       </c>
       <c r="I42" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J42">
         <v>0</v>
@@ -2230,7 +2230,7 @@
         <v>-1.11022302462515E-16</v>
       </c>
       <c r="I43" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J43">
         <v>0</v>
@@ -2262,7 +2262,7 @@
         <v>-1.11022302462515E-16</v>
       </c>
       <c r="I44" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J44">
         <v>0</v>
@@ -2294,7 +2294,7 @@
         <v>-1.11022302462515E-16</v>
       </c>
       <c r="I45" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J45">
         <v>0</v>
@@ -2326,7 +2326,7 @@
         <v>7.9999999999999905E-2</v>
       </c>
       <c r="I46" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J46">
         <v>0</v>
@@ -2358,7 +2358,7 @@
         <v>7.9999999999999905E-2</v>
       </c>
       <c r="I47" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J47">
         <v>0</v>
@@ -2390,7 +2390,7 @@
         <v>-1.11022302462515E-16</v>
       </c>
       <c r="I48" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J48">
         <v>0</v>
@@ -2422,7 +2422,7 @@
         <v>-1.11022302462515E-16</v>
       </c>
       <c r="I49" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J49">
         <v>0</v>
@@ -2454,7 +2454,7 @@
         <v>-1.11022302462515E-16</v>
       </c>
       <c r="I50" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J50">
         <v>0</v>
@@ -2486,7 +2486,7 @@
         <v>7.9999999999999905E-2</v>
       </c>
       <c r="I51" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J51">
         <v>0</v>
@@ -2518,7 +2518,7 @@
         <v>7.9999999999999905E-2</v>
       </c>
       <c r="I52" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J52">
         <v>0</v>

</xml_diff>